<commit_message>
Check Delete Button Enabled Test
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_DeleteButtonDisabledInGF_WithEvidence.xlsx
+++ b/src/main/resources/testdata/Check_DeleteButtonDisabledInGF_WithEvidence.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Data#</t>
   </si>
@@ -79,6 +79,114 @@
   </si>
   <si>
     <t>CA119664-CDNA//</t>
+  </si>
+  <si>
+    <t>gene_type</t>
+  </si>
+  <si>
+    <t>accessionNo</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>addSequence</t>
+  </si>
+  <si>
+    <t>proteindata</t>
+  </si>
+  <si>
+    <t>gfName</t>
+  </si>
+  <si>
+    <t>sourceSpecies</t>
+  </si>
+  <si>
+    <t>proteinSource</t>
+  </si>
+  <si>
+    <t>proteinAccessionNo</t>
+  </si>
+  <si>
+    <t>ProteinGiNo</t>
+  </si>
+  <si>
+    <t>proteinSymbol</t>
+  </si>
+  <si>
+    <t>proteinName</t>
+  </si>
+  <si>
+    <t>proteinSynonymsId</t>
+  </si>
+  <si>
+    <t>proteinDescription</t>
+  </si>
+  <si>
+    <t>orientationGD</t>
+  </si>
+  <si>
+    <t>sourceGS</t>
+  </si>
+  <si>
+    <t>accessionNoGS</t>
+  </si>
+  <si>
+    <t>1 caagtgccac tggctactag tgcaagtatg gctcgggtct ctgccaatgc agttgcactt
+       61 gttgcactcg tctccgttct tctcacgtat ggctgctgcg cccagtcgcc gctcaactac
+      121 accggctcct tggccaaatc ctccaaggct agctggtcat ggctccctgc caaggccaca
+      181 tggtacggcg cgcctaccgg cgccggtccc gatgacaacg gtggtgcttg cggctacaag
+      241 cacactaacc agtacccgtt catgtccatg acttcctgcg gcaacgagcc cctgttcaag
+      301 gacggcatgg gctgcggcgc ctgctaccag atacgatgcg tcaataacaa ggcctgctcc
+      361 ggcaagccgg agacggtcat gatcaccgac atgaactact accctgtggg caagtaccat
+      421 ttcgacctca gcggcacggc gttcggcgcc atggcgaagc ccggccagaa cgacaagctc
+      481 cgccacgccg gcattatcga catccagttc caaagggtgc catgcaatca tccgggcttg
+      541 aacgtgaact tccaggtcga gcggggctcc aaccccaact acctggccgt gctggtggag
+      601 ttcgcgaacc gggagggcac cgtggtgcag atggacctca tggagtcaag gaacggccgc
+      661 ccgacggggt actggacggc gatgcgccac tcgtggggcg ccatctggcg gatggactcc
+      721 aggcgccggc tgcagggccc cttctctctc cgcatccgca gcgaatccgg caagacgctg
+      781 gtggccaaac aagtcatccc ggccaactgg aggcccgaca cgaactaccg ttccaacgtc
+      841 cagttccgtt gattgctccg agcttccgat cgatcgacga agacgttgat taattcgg
+amakpgqndk lrhagiidiq  fqrvpcnhpg lnvnfqverg 181 snpnylavlv efanregtvv qmdlmesrng rptgywtamr hswgaiwrmd srrrlqgpfs 241 lrirsesgkt lvakqvipan wrpdtnyrsn vqfr</t>
+  </si>
+  <si>
+    <t>TaEXPB23</t>
+  </si>
+  <si>
+    <t>AY260547.prot</t>
+  </si>
+  <si>
+    <t>Avena sativa</t>
+  </si>
+  <si>
+    <t>OurProteinsource</t>
+  </si>
+  <si>
+    <t>AAAANNVV</t>
+  </si>
+  <si>
+    <t>AAP</t>
+  </si>
+  <si>
+    <t>SELENIUM_PROTEIN</t>
+  </si>
+  <si>
+    <t>ssaa</t>
+  </si>
+  <si>
+    <t>Test descrition</t>
+  </si>
+  <si>
+    <t>plus</t>
+  </si>
+  <si>
+    <t>AANV</t>
+  </si>
+  <si>
+    <t>selenium_assession</t>
+  </si>
+  <si>
+    <t>CGCCCGGGCAGGTGTACTATCCACTTAGCACAATAAAGAGAGAAAAACAAGGTAAGTTTAGTGAGTGTTCAAATGGCAGAAAACAAAGAAGAAGATGTTAAGCTTGGAGCTAACAAATTCAGAGAAACACAGCCATTAGGAACAGCTGCTCAAACAGACAAAGATTACAAAGAACCACCACCAGCTCCTTTGTTTGAACCAGGG</t>
   </si>
 </sst>
 </file>
@@ -114,8 +222,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,9 +547,19 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,10 +591,58 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -506,6 +675,54 @@
       </c>
       <c r="K2" t="s">
         <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>